<commit_message>
Reflect impact of abap2xlsx fix #1258
Fix #71
https://github.com/abap2xlsx/abap2xlsx/pull/1258
</commit_message>
<xml_diff>
--- a/src/zdemo_excel15_02.w3mi.data.xlsx
+++ b/src/zdemo_excel15_02.w3mi.data.xlsx
@@ -113,7 +113,7 @@
       <scheme val="major"/>
     </font>
   </fonts>
-  <fills count="18">
+  <fills count="19">
     <fill>
       <patternFill patternType="none">
         <bgColor indexed="64"/>
@@ -155,75 +155,85 @@
       </gradientFill>
     </fill>
     <fill>
+      <gradientFill type="path" bottom="1" top="1" right="1" left="1">
+        <stop position="0">
+          <color rgb="FFFFFFFF" indexed="64"/>
+        </stop>
+        <stop position="1">
+          <color rgb="FF0000FF"/>
+        </stop>
+      </gradientFill>
+    </fill>
+    <fill>
+      <gradientFill type="path" right="1" left="1">
+        <stop position="0">
+          <color rgb="FFFFFFFF" indexed="64"/>
+        </stop>
+        <stop position="1">
+          <color rgb="FF0000FF"/>
+        </stop>
+      </gradientFill>
+    </fill>
+    <fill>
+      <gradientFill degree="90">
+        <stop position="0">
+          <color rgb="FFFFFFFF" indexed="64"/>
+        </stop>
+        <stop position="1">
+          <color rgb="FF0000FF"/>
+        </stop>
+      </gradientFill>
+    </fill>
+    <fill>
+      <gradientFill degree="270">
+        <stop position="0">
+          <color rgb="FFFFFFFF" indexed="64"/>
+        </stop>
+        <stop position="1">
+          <color rgb="FF0000FF"/>
+        </stop>
+      </gradientFill>
+    </fill>
+    <fill>
+      <gradientFill degree="90">
+        <stop position="0">
+          <color rgb="FFFFFFFF" indexed="64"/>
+        </stop>
+        <stop position="0.5">
+          <color rgb="FF0000FF"/>
+        </stop>
+        <stop position="1">
+          <color rgb="FFFFFFFF" indexed="64"/>
+        </stop>
+      </gradientFill>
+    </fill>
+    <fill>
+      <gradientFill>
+        <stop position="0">
+          <color rgb="FFFFFFFF" indexed="64"/>
+        </stop>
+        <stop position="1">
+          <color rgb="FF0000FF"/>
+        </stop>
+      </gradientFill>
+    </fill>
+    <fill>
+      <gradientFill>
+        <stop position="0">
+          <color rgb="FF0000FF" indexed="64"/>
+        </stop>
+        <stop position="1">
+          <color rgb="FFFFFFFF"/>
+        </stop>
+      </gradientFill>
+    </fill>
+    <fill>
       <gradientFill type="path" bottom="0.5" top="0.5" right="0.5" left="0.5">
         <stop position="0">
           <color rgb="FFFFFFFF" indexed="64"/>
         </stop>
         <stop position="1">
           <color rgb="FF0000FF"/>
-        </stop>
-      </gradientFill>
-    </fill>
-    <fill>
-      <gradientFill type="path" right="1" left="1">
-        <stop position="0">
-          <color rgb="FFFFFFFF" indexed="64"/>
-        </stop>
-        <stop position="1">
-          <color rgb="FF0000FF"/>
-        </stop>
-      </gradientFill>
-    </fill>
-    <fill>
-      <gradientFill degree="90">
-        <stop position="0">
-          <color rgb="FFFFFFFF" indexed="64"/>
-        </stop>
-        <stop position="1">
-          <color rgb="FF0000FF"/>
-        </stop>
-      </gradientFill>
-    </fill>
-    <fill>
-      <gradientFill degree="270">
-        <stop position="0">
-          <color rgb="FFFFFFFF" indexed="64"/>
-        </stop>
-        <stop position="1">
-          <color rgb="FF0000FF"/>
-        </stop>
-      </gradientFill>
-    </fill>
-    <fill>
-      <gradientFill degree="90">
-        <stop position="0">
-          <color rgb="FFFFFFFF" indexed="64"/>
-        </stop>
-        <stop position="0.5">
-          <color rgb="FF0000FF"/>
-        </stop>
-        <stop position="1">
-          <color rgb="FFFFFFFF" indexed="64"/>
-        </stop>
-      </gradientFill>
-    </fill>
-    <fill>
-      <gradientFill>
-        <stop position="0">
-          <color rgb="FFFFFFFF" indexed="64"/>
-        </stop>
-        <stop position="1">
-          <color rgb="FF0000FF"/>
-        </stop>
-      </gradientFill>
-    </fill>
-    <fill>
-      <gradientFill>
-        <stop position="0">
-          <color rgb="FF0000FF" indexed="64"/>
-        </stop>
-        <stop position="1">
-          <color rgb="FFFFFFFF"/>
         </stop>
       </gradientFill>
     </fill>
@@ -323,7 +333,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="1" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -345,7 +355,8 @@
     <xf numFmtId="0" fontId="3" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -669,7 +680,7 @@
       </c>
     </row>
     <row r="9" spans="1:5">
-      <c r="B9" s="21" t="s">
+      <c r="B9" s="22" t="s">
         <v>5</v>
       </c>
     </row>
@@ -719,27 +730,27 @@
       </c>
     </row>
     <row r="19" spans="1:5" customHeight="1" ht="3.0000000000000000E+01">
-      <c r="C19" s="10" t="s">
+      <c r="C19" s="17" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="20" spans="1:5" customHeight="1" ht="3.0000000000000000E+01">
-      <c r="B20" s="17" t="s">
+      <c r="B20" s="18" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="21" spans="1:5" customHeight="1" ht="3.0000000000000000E+01">
-      <c r="C21" s="18" t="s">
+      <c r="C21" s="19" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="22" spans="1:5" customHeight="1" ht="3.0000000000000000E+01">
-      <c r="B22" s="19" t="s">
+      <c r="B22" s="20" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="23" spans="1:5" customHeight="1" ht="3.0000000000000000E+01">
-      <c r="C23" s="20" t="s">
+      <c r="C23" s="21" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Reflect impact of abap2xlsx fix #1258 (#72)
Fix #71
https://github.com/abap2xlsx/abap2xlsx/pull/1258
</commit_message>
<xml_diff>
--- a/src/zdemo_excel15_02.w3mi.data.xlsx
+++ b/src/zdemo_excel15_02.w3mi.data.xlsx
@@ -113,7 +113,7 @@
       <scheme val="major"/>
     </font>
   </fonts>
-  <fills count="18">
+  <fills count="19">
     <fill>
       <patternFill patternType="none">
         <bgColor indexed="64"/>
@@ -155,75 +155,85 @@
       </gradientFill>
     </fill>
     <fill>
+      <gradientFill type="path" bottom="1" top="1" right="1" left="1">
+        <stop position="0">
+          <color rgb="FFFFFFFF" indexed="64"/>
+        </stop>
+        <stop position="1">
+          <color rgb="FF0000FF"/>
+        </stop>
+      </gradientFill>
+    </fill>
+    <fill>
+      <gradientFill type="path" right="1" left="1">
+        <stop position="0">
+          <color rgb="FFFFFFFF" indexed="64"/>
+        </stop>
+        <stop position="1">
+          <color rgb="FF0000FF"/>
+        </stop>
+      </gradientFill>
+    </fill>
+    <fill>
+      <gradientFill degree="90">
+        <stop position="0">
+          <color rgb="FFFFFFFF" indexed="64"/>
+        </stop>
+        <stop position="1">
+          <color rgb="FF0000FF"/>
+        </stop>
+      </gradientFill>
+    </fill>
+    <fill>
+      <gradientFill degree="270">
+        <stop position="0">
+          <color rgb="FFFFFFFF" indexed="64"/>
+        </stop>
+        <stop position="1">
+          <color rgb="FF0000FF"/>
+        </stop>
+      </gradientFill>
+    </fill>
+    <fill>
+      <gradientFill degree="90">
+        <stop position="0">
+          <color rgb="FFFFFFFF" indexed="64"/>
+        </stop>
+        <stop position="0.5">
+          <color rgb="FF0000FF"/>
+        </stop>
+        <stop position="1">
+          <color rgb="FFFFFFFF" indexed="64"/>
+        </stop>
+      </gradientFill>
+    </fill>
+    <fill>
+      <gradientFill>
+        <stop position="0">
+          <color rgb="FFFFFFFF" indexed="64"/>
+        </stop>
+        <stop position="1">
+          <color rgb="FF0000FF"/>
+        </stop>
+      </gradientFill>
+    </fill>
+    <fill>
+      <gradientFill>
+        <stop position="0">
+          <color rgb="FF0000FF" indexed="64"/>
+        </stop>
+        <stop position="1">
+          <color rgb="FFFFFFFF"/>
+        </stop>
+      </gradientFill>
+    </fill>
+    <fill>
       <gradientFill type="path" bottom="0.5" top="0.5" right="0.5" left="0.5">
         <stop position="0">
           <color rgb="FFFFFFFF" indexed="64"/>
         </stop>
         <stop position="1">
           <color rgb="FF0000FF"/>
-        </stop>
-      </gradientFill>
-    </fill>
-    <fill>
-      <gradientFill type="path" right="1" left="1">
-        <stop position="0">
-          <color rgb="FFFFFFFF" indexed="64"/>
-        </stop>
-        <stop position="1">
-          <color rgb="FF0000FF"/>
-        </stop>
-      </gradientFill>
-    </fill>
-    <fill>
-      <gradientFill degree="90">
-        <stop position="0">
-          <color rgb="FFFFFFFF" indexed="64"/>
-        </stop>
-        <stop position="1">
-          <color rgb="FF0000FF"/>
-        </stop>
-      </gradientFill>
-    </fill>
-    <fill>
-      <gradientFill degree="270">
-        <stop position="0">
-          <color rgb="FFFFFFFF" indexed="64"/>
-        </stop>
-        <stop position="1">
-          <color rgb="FF0000FF"/>
-        </stop>
-      </gradientFill>
-    </fill>
-    <fill>
-      <gradientFill degree="90">
-        <stop position="0">
-          <color rgb="FFFFFFFF" indexed="64"/>
-        </stop>
-        <stop position="0.5">
-          <color rgb="FF0000FF"/>
-        </stop>
-        <stop position="1">
-          <color rgb="FFFFFFFF" indexed="64"/>
-        </stop>
-      </gradientFill>
-    </fill>
-    <fill>
-      <gradientFill>
-        <stop position="0">
-          <color rgb="FFFFFFFF" indexed="64"/>
-        </stop>
-        <stop position="1">
-          <color rgb="FF0000FF"/>
-        </stop>
-      </gradientFill>
-    </fill>
-    <fill>
-      <gradientFill>
-        <stop position="0">
-          <color rgb="FF0000FF" indexed="64"/>
-        </stop>
-        <stop position="1">
-          <color rgb="FFFFFFFF"/>
         </stop>
       </gradientFill>
     </fill>
@@ -323,7 +333,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="1" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -345,7 +355,8 @@
     <xf numFmtId="0" fontId="3" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -669,7 +680,7 @@
       </c>
     </row>
     <row r="9" spans="1:5">
-      <c r="B9" s="21" t="s">
+      <c r="B9" s="22" t="s">
         <v>5</v>
       </c>
     </row>
@@ -719,27 +730,27 @@
       </c>
     </row>
     <row r="19" spans="1:5" customHeight="1" ht="3.0000000000000000E+01">
-      <c r="C19" s="10" t="s">
+      <c r="C19" s="17" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="20" spans="1:5" customHeight="1" ht="3.0000000000000000E+01">
-      <c r="B20" s="17" t="s">
+      <c r="B20" s="18" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="21" spans="1:5" customHeight="1" ht="3.0000000000000000E+01">
-      <c r="C21" s="18" t="s">
+      <c r="C21" s="19" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="22" spans="1:5" customHeight="1" ht="3.0000000000000000E+01">
-      <c r="B22" s="19" t="s">
+      <c r="B22" s="20" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="23" spans="1:5" customHeight="1" ht="3.0000000000000000E+01">
-      <c r="C23" s="20" t="s">
+      <c r="C23" s="21" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update excels in web repo (ZDEMO_EXCEL_CHECKER)
</commit_message>
<xml_diff>
--- a/src/zdemo_excel15_02.w3mi.data.xlsx
+++ b/src/zdemo_excel15_02.w3mi.data.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
   <si>
     <t>Bold text</t>
   </si>
@@ -72,6 +72,9 @@
   </si>
   <si>
     <t>horizontalb</t>
+  </si>
+  <si>
+    <t>little off fromCenter</t>
   </si>
   <si>
     <t>vertical</t>
@@ -113,7 +116,7 @@
       <scheme val="major"/>
     </font>
   </fonts>
-  <fills count="19">
+  <fills count="20">
     <fill>
       <patternFill patternType="none">
         <bgColor indexed="64"/>
@@ -287,6 +290,16 @@
       <patternFill patternType="solid">
         <fgColor indexed="16"/>
       </patternFill>
+    </fill>
+    <fill>
+      <gradientFill type="path" bottom="0.4" top="0.3" right="0.4" left="0.3">
+        <stop position="0">
+          <color rgb="FFFFFFFF" indexed="64"/>
+        </stop>
+        <stop position="1">
+          <color rgb="FF0000FF"/>
+        </stop>
+      </gradientFill>
     </fill>
   </fills>
   <borders count="3">
@@ -333,7 +346,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="1" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -357,6 +370,7 @@
     <xf numFmtId="0" fontId="3" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -721,17 +735,20 @@
     </row>
     <row r="17" spans="1:5" customHeight="1" ht="3.0000000000000000E+01">
       <c r="C17" s="15" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="18" spans="1:5" customHeight="1" ht="3.0000000000000000E+01">
       <c r="B18" s="16" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="19" spans="1:5" customHeight="1" ht="3.0000000000000000E+01">
       <c r="C19" s="17" t="s">
         <v>15</v>
+      </c>
+      <c r="E19" s="23" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="20" spans="1:5" customHeight="1" ht="3.0000000000000000E+01">

</xml_diff>

<commit_message>
ZDEMO_EXCEL2: add change_cell_style showcase (#74)
* add change_cell_style showcase

fixes 73

needed to test https://github.com/abap2xlsx/abap2xlsx/pull/1260

* update excels in web repo (ZDEMO_EXCEL_CHECKER)
</commit_message>
<xml_diff>
--- a/src/zdemo_excel15_02.w3mi.data.xlsx
+++ b/src/zdemo_excel15_02.w3mi.data.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
   <si>
     <t>Bold text</t>
   </si>
@@ -72,6 +72,9 @@
   </si>
   <si>
     <t>horizontalb</t>
+  </si>
+  <si>
+    <t>little off fromCenter</t>
   </si>
   <si>
     <t>vertical</t>
@@ -113,7 +116,7 @@
       <scheme val="major"/>
     </font>
   </fonts>
-  <fills count="19">
+  <fills count="20">
     <fill>
       <patternFill patternType="none">
         <bgColor indexed="64"/>
@@ -287,6 +290,16 @@
       <patternFill patternType="solid">
         <fgColor indexed="16"/>
       </patternFill>
+    </fill>
+    <fill>
+      <gradientFill type="path" bottom="0.4" top="0.3" right="0.4" left="0.3">
+        <stop position="0">
+          <color rgb="FFFFFFFF" indexed="64"/>
+        </stop>
+        <stop position="1">
+          <color rgb="FF0000FF"/>
+        </stop>
+      </gradientFill>
     </fill>
   </fills>
   <borders count="3">
@@ -333,7 +346,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="1" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -357,6 +370,7 @@
     <xf numFmtId="0" fontId="3" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -721,17 +735,20 @@
     </row>
     <row r="17" spans="1:5" customHeight="1" ht="3.0000000000000000E+01">
       <c r="C17" s="15" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="18" spans="1:5" customHeight="1" ht="3.0000000000000000E+01">
       <c r="B18" s="16" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="19" spans="1:5" customHeight="1" ht="3.0000000000000000E+01">
       <c r="C19" s="17" t="s">
         <v>15</v>
+      </c>
+      <c r="E19" s="23" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="20" spans="1:5" customHeight="1" ht="3.0000000000000000E+01">

</xml_diff>